<commit_message>
thêm công thức đếm số thứ tự
</commit_message>
<xml_diff>
--- a/Mau.xlsx
+++ b/Mau.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lichvu\Documents\GitHub\nvexcel-react\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\nvexcel-react\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{04CE5CE3-F535-4A3B-B79B-90041E2BC7B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CF2177-75B3-43D2-AC71-980977544BF0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{257AB335-7A00-4FE0-AC24-7A3D3259B442}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{257AB335-7A00-4FE0-AC24-7A3D3259B442}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mẫu khối lượng" sheetId="15" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>STT</t>
   </si>
@@ -73,6 +74,15 @@
   </si>
   <si>
     <t>Địa điểm:</t>
+  </si>
+  <si>
+    <t>BẢNG MẪU KHỐI LƯỢNG CÔNG TRÌNH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Công trình: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Địa điểm: </t>
   </si>
 </sst>
 </file>
@@ -127,12 +137,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +457,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -467,99 +477,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4602ACF9-4DAE-4852-BB22-72E979E4BACA}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
     <col min="3" max="3" width="12" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="22.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="30.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="1"/>
+    <col min="11" max="11" width="22.109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -578,41 +588,49 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
+        <f>A7+1</f>
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
+        <f t="shared" ref="A9:A15" si="0">A8+1</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -625,4 +643,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47BBA79-C2FC-4148-A7EE-2238253760A1}">
+  <dimension ref="A1:L5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="b">
+        <f ca="1">IF(B8&gt;INDIRECT("RC[-1]",0),TRUE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:J1048576">
+    <cfRule type="expression" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>